<commit_message>
Website Content Update , Stundenaufzeichnung update
New Content on Website, updated record of working hours
</commit_message>
<xml_diff>
--- a/Dokumente/Stundenaufzeichnung.xlsx
+++ b/Dokumente/Stundenaufzeichnung.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yimne/Documents/4CHIF/SYP/Projekt/webshop-jasmin/Dokumente/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\willi\Desktop\Schule\SYP\Project Repo\webshop-jasmin\Dokumente\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AD7625D-47C8-6E46-B563-1E9B418893C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38DBCF91-E061-4A6E-B1A2-D0D7ADFE2E9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sprintreview" sheetId="3" r:id="rId1"/>
@@ -25,9 +25,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -36,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="32">
   <si>
     <t>Stundenaufzeichnung:</t>
   </si>
@@ -110,12 +108,6 @@
     <t>Produktliste überarbeitet</t>
   </si>
   <si>
-    <t>Bilder von Produkten aufgenommen</t>
-  </si>
-  <si>
-    <t>Hugo runtergeladen und mit einer demo Website getestet</t>
-  </si>
-  <si>
     <t>Website mit Hugo konfigurieren</t>
   </si>
   <si>
@@ -129,6 +121,15 @@
   </si>
   <si>
     <t>Bilder bearbeitet</t>
+  </si>
+  <si>
+    <t>Sich mit Hugo auseinandersetzen(test website, funktionen lernen etc)</t>
+  </si>
+  <si>
+    <t>Produktbilder aufnehmen</t>
+  </si>
+  <si>
+    <t>Website konfigurieren</t>
   </si>
 </sst>
 </file>
@@ -191,7 +192,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -222,6 +223,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -504,16 +506,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79A89811-AC7A-4BDB-875B-6F9F15541B52}">
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="22.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.65">
       <c r="A1" s="11" t="s">
         <v>21</v>
       </c>
@@ -521,19 +523,19 @@
       <c r="C1" s="7"/>
       <c r="D1" s="7"/>
     </row>
-    <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.65">
       <c r="A2" s="11"/>
       <c r="B2" s="11"/>
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
     </row>
-    <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.65">
       <c r="A3" s="6"/>
       <c r="B3" s="6"/>
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>19</v>
       </c>
@@ -542,43 +544,45 @@
         <v>0.84722222222222232</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="5"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B5" s="5">
+        <v>2.53125</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B6" s="5"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B7" s="5"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B8" s="5"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B9" s="5"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B10" s="5"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B11" s="5"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B12" s="5"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B13" s="5"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B14" s="5"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B15" s="5"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B16" s="5"/>
     </row>
   </sheetData>
@@ -594,34 +598,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M3" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="S12" sqref="S12"/>
+    <sheetView zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="57.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="57.6328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.6328125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="56.1640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="60.83203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="48.33203125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="56.1796875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.6328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="60.81640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.6328125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.453125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="48.36328125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.6328125" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="7" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="14.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -635,7 +639,7 @@
       <c r="K1" s="11"/>
       <c r="L1" s="11"/>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A2" s="12"/>
       <c r="B2" s="12"/>
       <c r="C2" s="12"/>
@@ -645,7 +649,7 @@
       <c r="K2" s="11"/>
       <c r="L2" s="11"/>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -695,7 +699,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -745,7 +749,7 @@
         <v>0.11805555555555557</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.35">
       <c r="B6" s="2">
         <v>44549</v>
       </c>
@@ -784,63 +788,63 @@
       </c>
       <c r="X6" s="3"/>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.35">
       <c r="B7" s="2">
-        <v>44564</v>
+        <v>44558</v>
       </c>
       <c r="C7" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="D7" s="3">
-        <v>0.16666666666666666</v>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="G7" s="2">
-        <v>44900</v>
+        <v>44558</v>
       </c>
       <c r="H7" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="I7" s="3">
-        <v>0.20833333333333334</v>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="L7" s="2">
         <v>44558</v>
       </c>
       <c r="M7" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="N7" s="9">
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="Q7" s="2">
-        <v>44566</v>
+        <v>44558</v>
       </c>
       <c r="R7" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="S7" s="3">
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="X7" s="3"/>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.35">
       <c r="B8" s="2">
-        <v>44566</v>
+        <v>44564</v>
       </c>
       <c r="C8" t="s">
         <v>16</v>
       </c>
       <c r="D8" s="3">
-        <v>0.20833333333333334</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="G8" s="2">
-        <v>44568</v>
+        <v>44564</v>
       </c>
       <c r="H8" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="I8" s="3">
-        <v>0.15625</v>
+        <v>0.125</v>
       </c>
       <c r="L8" s="2">
         <v>44564</v>
@@ -852,46 +856,46 @@
         <v>0.125</v>
       </c>
       <c r="Q8" s="2">
-        <v>44568</v>
+        <v>44566</v>
       </c>
       <c r="R8" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="S8" s="3">
-        <v>0.15625</v>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="X8" s="3"/>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.35">
       <c r="B9" s="2">
-        <v>44568</v>
+        <v>44566</v>
       </c>
       <c r="C9" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="D9" s="3">
-        <v>0.15625</v>
+        <v>0.20833333333333334</v>
       </c>
       <c r="G9" s="2">
-        <v>44570</v>
+        <v>44900</v>
       </c>
       <c r="H9" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="I9" s="3">
-        <v>0.1875</v>
+        <v>0.20833333333333334</v>
       </c>
       <c r="L9" s="2">
         <v>44566</v>
       </c>
       <c r="M9" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="N9" s="3">
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="Q9" s="2">
-        <v>44570</v>
+        <v>44567</v>
       </c>
       <c r="R9" t="s">
         <v>30</v>
@@ -901,162 +905,209 @@
       </c>
       <c r="X9" s="3"/>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.35">
       <c r="B10" s="2">
-        <v>44570</v>
+        <v>44568</v>
       </c>
       <c r="C10" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="D10" s="3">
-        <v>6.25E-2</v>
-      </c>
-      <c r="I10" s="3"/>
+        <v>0.15625</v>
+      </c>
+      <c r="G10" s="2">
+        <v>44568</v>
+      </c>
+      <c r="H10" t="s">
+        <v>24</v>
+      </c>
+      <c r="I10" s="3">
+        <v>0.15625</v>
+      </c>
       <c r="L10" s="2">
         <v>44567</v>
       </c>
       <c r="M10" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="N10" s="3">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="S10" s="3"/>
+      <c r="Q10" s="2">
+        <v>44568</v>
+      </c>
+      <c r="R10" t="s">
+        <v>24</v>
+      </c>
+      <c r="S10" s="3">
+        <v>0.15625</v>
+      </c>
       <c r="X10" s="3"/>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="D11" s="3"/>
-      <c r="I11" s="3"/>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="B11" s="2">
+        <v>44570</v>
+      </c>
+      <c r="C11" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" s="3">
+        <v>0.125</v>
+      </c>
+      <c r="G11" s="2">
+        <v>44570</v>
+      </c>
+      <c r="H11" t="s">
+        <v>25</v>
+      </c>
+      <c r="I11" s="3">
+        <v>0.1875</v>
+      </c>
       <c r="L11" s="2">
         <v>44570</v>
       </c>
       <c r="M11" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="N11" s="3">
         <v>0.16666666666666666</v>
       </c>
-      <c r="S11" s="3"/>
+      <c r="Q11" s="2">
+        <v>44570</v>
+      </c>
+      <c r="R11" t="s">
+        <v>28</v>
+      </c>
+      <c r="S11" s="3">
+        <v>8.3333333333333329E-2</v>
+      </c>
       <c r="X11" s="3"/>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.35">
       <c r="D12" s="3"/>
       <c r="I12" s="3"/>
       <c r="N12" s="3"/>
       <c r="S12" s="3"/>
       <c r="X12" s="3"/>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.35">
       <c r="D13" s="3"/>
       <c r="I13" s="3"/>
       <c r="N13" s="3"/>
       <c r="S13" s="3"/>
       <c r="X13" s="3"/>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A14" s="14"/>
+      <c r="B14" s="14"/>
       <c r="D14" s="3"/>
       <c r="I14" s="3"/>
       <c r="N14" s="3"/>
       <c r="S14" s="3"/>
       <c r="X14" s="3"/>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.35">
       <c r="D15" s="3"/>
       <c r="I15" s="3"/>
       <c r="N15" s="3"/>
       <c r="S15" s="3"/>
       <c r="X15" s="3"/>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.35">
       <c r="D16" s="3"/>
       <c r="I16" s="3"/>
       <c r="N16" s="3"/>
       <c r="S16" s="3"/>
       <c r="X16" s="3"/>
     </row>
-    <row r="17" spans="4:24" x14ac:dyDescent="0.2">
+    <row r="17" spans="4:24" x14ac:dyDescent="0.35">
       <c r="D17" s="3"/>
       <c r="I17" s="3"/>
       <c r="N17" s="3"/>
       <c r="S17" s="3"/>
       <c r="X17" s="3"/>
     </row>
-    <row r="18" spans="4:24" x14ac:dyDescent="0.2">
+    <row r="18" spans="4:24" x14ac:dyDescent="0.35">
       <c r="D18" s="3"/>
       <c r="I18" s="3"/>
       <c r="N18" s="3"/>
       <c r="S18" s="3"/>
       <c r="X18" s="3"/>
     </row>
-    <row r="19" spans="4:24" x14ac:dyDescent="0.2">
+    <row r="19" spans="4:24" x14ac:dyDescent="0.35">
       <c r="D19" s="3"/>
       <c r="I19" s="3"/>
       <c r="N19" s="3"/>
       <c r="S19" s="3"/>
       <c r="X19" s="3"/>
     </row>
-    <row r="20" spans="4:24" x14ac:dyDescent="0.2">
+    <row r="20" spans="4:24" x14ac:dyDescent="0.35">
       <c r="D20" s="3"/>
       <c r="I20" s="3"/>
       <c r="N20" s="3"/>
       <c r="S20" s="3"/>
       <c r="X20" s="3"/>
     </row>
-    <row r="21" spans="4:24" x14ac:dyDescent="0.2">
+    <row r="21" spans="4:24" x14ac:dyDescent="0.35">
       <c r="D21" s="3"/>
       <c r="I21" s="3"/>
       <c r="N21" s="3"/>
       <c r="S21" s="3"/>
       <c r="X21" s="3"/>
     </row>
-    <row r="22" spans="4:24" x14ac:dyDescent="0.2">
+    <row r="22" spans="4:24" x14ac:dyDescent="0.35">
       <c r="D22" s="3"/>
       <c r="I22" s="3"/>
       <c r="N22" s="3"/>
       <c r="S22" s="3"/>
       <c r="X22" s="3"/>
     </row>
-    <row r="23" spans="4:24" x14ac:dyDescent="0.2">
+    <row r="23" spans="4:24" x14ac:dyDescent="0.35">
       <c r="D23" s="3"/>
       <c r="I23" s="3"/>
       <c r="N23" s="3"/>
       <c r="S23" s="3"/>
       <c r="X23" s="3"/>
     </row>
-    <row r="24" spans="4:24" x14ac:dyDescent="0.2">
+    <row r="24" spans="4:24" x14ac:dyDescent="0.35">
       <c r="D24" s="3"/>
       <c r="I24" s="3"/>
       <c r="N24" s="3"/>
       <c r="S24" s="3"/>
       <c r="X24" s="3"/>
     </row>
-    <row r="25" spans="4:24" x14ac:dyDescent="0.2">
+    <row r="25" spans="4:24" x14ac:dyDescent="0.35">
       <c r="D25" s="3"/>
       <c r="I25" s="3"/>
       <c r="N25" s="3"/>
       <c r="S25" s="3"/>
       <c r="X25" s="3"/>
     </row>
-    <row r="26" spans="4:24" x14ac:dyDescent="0.2">
+    <row r="26" spans="4:24" x14ac:dyDescent="0.35">
       <c r="D26" s="3"/>
       <c r="I26" s="3"/>
       <c r="N26" s="3"/>
       <c r="S26" s="3"/>
       <c r="X26" s="3"/>
     </row>
-    <row r="27" spans="4:24" x14ac:dyDescent="0.2">
+    <row r="27" spans="4:24" x14ac:dyDescent="0.35">
       <c r="D27" s="3"/>
+      <c r="I27" s="3"/>
+      <c r="S27" s="3"/>
       <c r="X27" s="3"/>
     </row>
-    <row r="28" spans="4:24" x14ac:dyDescent="0.2">
+    <row r="28" spans="4:24" x14ac:dyDescent="0.35">
       <c r="D28" s="3"/>
+      <c r="I28" s="3"/>
+      <c r="S28" s="3"/>
       <c r="X28" s="3"/>
     </row>
-    <row r="29" spans="4:24" x14ac:dyDescent="0.2">
+    <row r="29" spans="4:24" x14ac:dyDescent="0.35">
       <c r="D29" s="3"/>
       <c r="X29" s="3"/>
     </row>
-    <row r="30" spans="4:24" x14ac:dyDescent="0.2">
+    <row r="30" spans="4:24" x14ac:dyDescent="0.35">
+      <c r="D30" s="3"/>
       <c r="X30" s="3"/>
     </row>
   </sheetData>
@@ -1074,15 +1125,15 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="13" t="s">
         <v>18</v>
       </c>
@@ -1090,19 +1141,19 @@
       <c r="C1" s="13"/>
       <c r="D1" s="13"/>
     </row>
-    <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="13"/>
       <c r="B2" s="13"/>
       <c r="C2" s="13"/>
       <c r="D2" s="13"/>
     </row>
-    <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.65">
       <c r="A3" s="8"/>
       <c r="B3" s="8"/>
       <c r="C3" s="8"/>
       <c r="D3" s="8"/>
     </row>
-    <row r="4" spans="1:4" ht="21" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -1111,25 +1162,25 @@
       </c>
       <c r="C4" s="4"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="5">
-        <f>SUM(Stundenaufzeichnung!D5:D26)</f>
-        <v>0.80902777777777779</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+        <f>SUM(Stundenaufzeichnung!D5:D27)</f>
+        <v>0.95486111111111116</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="5">
-        <f>SUM(Stundenaufzeichnung!I3:I17)</f>
-        <v>0.82291666666666674</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+        <f>SUM(Stundenaufzeichnung!I3:I19)</f>
+        <v>1.03125</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
@@ -1138,16 +1189,16 @@
         <v>0.70833333333333326</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B8" s="5">
-        <f>SUM(Stundenaufzeichnung!S3:S24)</f>
-        <v>0.51736111111111116</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+        <f>SUM(Stundenaufzeichnung!S3:S26)</f>
+        <v>0.68402777777777779</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="1"/>
       <c r="B9" s="10"/>
     </row>

</xml_diff>